<commit_message>
Student, module, groups assignment
</commit_message>
<xml_diff>
--- a/src/main/resources/file/ProgrammeDetails.xlsx
+++ b/src/main/resources/file/ProgrammeDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3738771-0F8C-4A09-8872-8A8F1C84D14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B2D466-86F5-4C1F-8AA9-9288E0112CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A2388C57-8624-4C34-9FA2-70B15EFCE8BC}"/>
   </bookViews>
@@ -611,7 +611,7 @@
   <dimension ref="A1:D148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136"/>
+      <selection activeCell="A120" sqref="A120:XFD148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Refactor: Group student based on semester
</commit_message>
<xml_diff>
--- a/src/main/resources/file/ProgrammeDetails.xlsx
+++ b/src/main/resources/file/ProgrammeDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B2D466-86F5-4C1F-8AA9-9288E0112CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169A87CA-2F07-4E54-B848-D707506E4B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A2388C57-8624-4C34-9FA2-70B15EFCE8BC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="66">
   <si>
     <t>Programme ID</t>
   </si>
@@ -137,9 +137,6 @@
     <t>WEB2202</t>
   </si>
   <si>
-    <t>BSC</t>
-  </si>
-  <si>
     <t>CSC1024</t>
   </si>
   <si>
@@ -231,6 +228,12 @@
   </si>
   <si>
     <t>End Year</t>
+  </si>
+  <si>
+    <t>BCS</t>
+  </si>
+  <si>
+    <t>ENG1044</t>
   </si>
 </sst>
 </file>
@@ -608,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4767327-0D20-4F94-B637-A0466E39E7A8}">
-  <dimension ref="A1:D148"/>
+  <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120:XFD148"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,13 +630,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -674,7 +677,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <v>2022</v>
@@ -685,7 +688,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>2022</v>
@@ -696,7 +699,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>2022</v>
@@ -707,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>2022</v>
@@ -718,7 +721,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>2022</v>
@@ -729,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>2022</v>
@@ -740,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>2022</v>
@@ -751,7 +754,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>2022</v>
@@ -762,7 +765,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>2022</v>
@@ -773,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="C14">
         <v>2022</v>
@@ -784,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>2022</v>
@@ -795,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>2022</v>
@@ -806,7 +809,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>2022</v>
@@ -817,7 +820,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>2022</v>
@@ -828,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>2022</v>
@@ -839,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>2022</v>
@@ -850,7 +853,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <v>2022</v>
@@ -861,7 +864,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C22">
         <v>2022</v>
@@ -872,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C23">
         <v>2022</v>
@@ -883,7 +886,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C24">
         <v>2022</v>
@@ -894,7 +897,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25">
         <v>2022</v>
@@ -905,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26">
         <v>2022</v>
@@ -916,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C27">
         <v>2022</v>
@@ -927,7 +930,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28">
         <v>2022</v>
@@ -938,7 +941,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C29">
         <v>2022</v>
@@ -949,7 +952,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C30">
         <v>2022</v>
@@ -960,7 +963,7 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31">
         <v>2022</v>
@@ -971,7 +974,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C32">
         <v>2022</v>
@@ -982,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C33">
         <v>2022</v>
@@ -990,10 +993,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="C34">
         <v>2022</v>
@@ -1001,10 +1004,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C35">
         <v>2022</v>
@@ -1012,10 +1015,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C36">
         <v>2022</v>
@@ -1023,10 +1026,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" t="s">
         <v>33</v>
-      </c>
-      <c r="B37" t="s">
-        <v>35</v>
       </c>
       <c r="C37">
         <v>2022</v>
@@ -1034,10 +1037,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38">
         <v>2022</v>
@@ -1045,10 +1048,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C39">
         <v>2022</v>
@@ -1056,10 +1059,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40">
         <v>2022</v>
@@ -1067,10 +1070,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C41">
         <v>2022</v>
@@ -1078,10 +1081,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C42">
         <v>2022</v>
@@ -1089,10 +1092,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C43">
         <v>2022</v>
@@ -1100,10 +1103,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C44">
         <v>2022</v>
@@ -1111,10 +1114,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C45">
         <v>2022</v>
@@ -1122,10 +1125,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C46">
         <v>2022</v>
@@ -1133,10 +1136,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C47">
         <v>2022</v>
@@ -1144,10 +1147,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C48">
         <v>2022</v>
@@ -1155,10 +1158,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C49">
         <v>2022</v>
@@ -1166,10 +1169,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="C50">
         <v>2022</v>
@@ -1177,10 +1180,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C51">
         <v>2022</v>
@@ -1188,10 +1191,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C52">
         <v>2022</v>
@@ -1199,10 +1202,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C53">
         <v>2022</v>
@@ -1210,10 +1213,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C54">
         <v>2022</v>
@@ -1221,10 +1224,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C55">
         <v>2022</v>
@@ -1232,10 +1235,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C56">
         <v>2022</v>
@@ -1243,10 +1246,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C57">
         <v>2022</v>
@@ -1254,10 +1257,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C58">
         <v>2022</v>
@@ -1265,10 +1268,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B59" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C59">
         <v>2022</v>
@@ -1276,10 +1279,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C60">
         <v>2022</v>
@@ -1287,10 +1290,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C61">
         <v>2022</v>
@@ -1298,10 +1301,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C62">
         <v>2022</v>
@@ -1309,10 +1312,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C63">
         <v>2022</v>
@@ -1320,10 +1323,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C64">
         <v>2022</v>
@@ -1331,10 +1334,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C65">
         <v>2022</v>
@@ -1342,10 +1345,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C66">
         <v>2022</v>
@@ -1353,10 +1356,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C67">
         <v>2022</v>
@@ -1364,10 +1367,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C68">
         <v>2022</v>
@@ -1375,10 +1378,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" t="s">
         <v>42</v>
-      </c>
-      <c r="B69" t="s">
-        <v>45</v>
       </c>
       <c r="C69">
         <v>2022</v>
@@ -1386,10 +1389,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B70" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C70">
         <v>2022</v>
@@ -1397,10 +1400,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C71">
         <v>2022</v>
@@ -1408,10 +1411,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B72" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C72">
         <v>2022</v>
@@ -1419,10 +1422,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B73" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C73">
         <v>2022</v>
@@ -1430,24 +1433,21 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B74" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="C74">
         <v>2022</v>
-      </c>
-      <c r="D74">
-        <v>2023</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B75" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C75">
         <v>2022</v>
@@ -1455,49 +1455,46 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B76" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="C76">
         <v>2022</v>
-      </c>
-      <c r="D76">
-        <v>2023</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B77" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C77">
         <v>2022</v>
-      </c>
-      <c r="D77">
-        <v>2023</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B78" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C78">
-        <v>2024</v>
+        <v>2022</v>
+      </c>
+      <c r="D78">
+        <v>2023</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B79" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C79">
         <v>2022</v>
@@ -1505,43 +1502,49 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B80" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C80">
         <v>2022</v>
+      </c>
+      <c r="D80">
+        <v>2023</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B81" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C81">
         <v>2022</v>
+      </c>
+      <c r="D81">
+        <v>2023</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B82" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C82">
-        <v>2022</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B83" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C83">
         <v>2022</v>
@@ -1549,10 +1552,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B84" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C84">
         <v>2022</v>
@@ -1560,21 +1563,21 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C85">
-        <v>2024</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B86" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C86">
         <v>2022</v>
@@ -1582,10 +1585,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B87" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C87">
         <v>2022</v>
@@ -1593,24 +1596,21 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B88" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C88">
         <v>2022</v>
-      </c>
-      <c r="D88">
-        <v>2023</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B89" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="C89">
         <v>2024</v>
@@ -1618,10 +1618,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B90" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C90">
         <v>2022</v>
@@ -1629,10 +1629,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B91" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C91">
         <v>2022</v>
@@ -1640,10 +1640,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B92" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C92">
         <v>2022</v>
@@ -1651,32 +1651,35 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B93" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C93">
         <v>2022</v>
+      </c>
+      <c r="D93">
+        <v>2023</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B94" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="C94">
-        <v>2022</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B95" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C95">
         <v>2022</v>
@@ -1684,35 +1687,32 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B96" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="C96">
         <v>2022</v>
-      </c>
-      <c r="D96">
-        <v>2023</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B97" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="C97">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B98" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C98">
         <v>2022</v>
@@ -1720,10 +1720,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B99" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C99">
         <v>2022</v>
@@ -1731,10 +1731,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B100" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="C100">
         <v>2022</v>
@@ -1742,57 +1742,57 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B101" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C101">
-        <v>2024</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>49</v>
+      </c>
+      <c r="B102" t="s">
         <v>50</v>
       </c>
-      <c r="B102" t="s">
-        <v>17</v>
-      </c>
       <c r="C102">
         <v>2022</v>
+      </c>
+      <c r="D102">
+        <v>2023</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B103" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C103">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B104" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C104">
         <v>2022</v>
-      </c>
-      <c r="D104">
-        <v>2023</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B105" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C105">
         <v>2022</v>
@@ -1800,10 +1800,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B106" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C106">
         <v>2022</v>
@@ -1811,21 +1811,21 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B107" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C107">
-        <v>2022</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B108" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C108">
         <v>2022</v>
@@ -1833,10 +1833,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B109" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C109">
         <v>2024</v>
@@ -1844,21 +1844,24 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B110" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C110">
         <v>2022</v>
+      </c>
+      <c r="D110">
+        <v>2023</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B111" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C111">
         <v>2022</v>
@@ -1866,10 +1869,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B112" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C112">
         <v>2022</v>
@@ -1877,10 +1880,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B113" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C113">
         <v>2022</v>
@@ -1888,10 +1891,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B114" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="C114">
         <v>2022</v>
@@ -1899,21 +1902,21 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B115" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C115">
-        <v>2022</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B116" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="C116">
         <v>2022</v>
@@ -1921,10 +1924,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B117" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C117">
         <v>2022</v>
@@ -1932,10 +1935,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B118" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C118">
         <v>2022</v>
@@ -1943,24 +1946,21 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B119" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C119">
         <v>2022</v>
-      </c>
-      <c r="D119">
-        <v>2023</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B120" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C120">
         <v>2022</v>
@@ -1968,10 +1968,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B121" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C121">
         <v>2022</v>
@@ -1979,74 +1979,68 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B122" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="C122">
         <v>2022</v>
-      </c>
-      <c r="D122">
-        <v>2023</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B123" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C123">
         <v>2022</v>
-      </c>
-      <c r="D123">
-        <v>2023</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B124" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C124">
-        <v>2024</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B125" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C125">
-        <v>2024</v>
+        <v>2022</v>
+      </c>
+      <c r="D125">
+        <v>2023</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B126" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C126">
         <v>2022</v>
-      </c>
-      <c r="D126">
-        <v>2023</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B127" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C127">
         <v>2022</v>
@@ -2054,10 +2048,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B128" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C128">
         <v>2022</v>
@@ -2068,57 +2062,60 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B129" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C129">
-        <v>2024</v>
+        <v>2022</v>
+      </c>
+      <c r="D129">
+        <v>2023</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>55</v>
+      </c>
+      <c r="B130" t="s">
         <v>56</v>
       </c>
-      <c r="B130" t="s">
-        <v>58</v>
-      </c>
       <c r="C130">
-        <v>2022</v>
-      </c>
-      <c r="D130">
-        <v>2023</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B131" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C131">
-        <v>2022</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B132" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="C132">
         <v>2022</v>
+      </c>
+      <c r="D132">
+        <v>2023</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B133" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="C133">
         <v>2022</v>
@@ -2126,10 +2123,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B134" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C134">
         <v>2022</v>
@@ -2137,43 +2134,49 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B135" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C135">
         <v>2022</v>
+      </c>
+      <c r="D135">
+        <v>2023</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B136" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C136">
-        <v>2022</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B137" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="C137">
         <v>2022</v>
+      </c>
+      <c r="D137">
+        <v>2023</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B138" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C138">
         <v>2022</v>
@@ -2181,24 +2184,21 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B139" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="C139">
         <v>2022</v>
-      </c>
-      <c r="D139">
-        <v>2023</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B140" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C140">
         <v>2022</v>
@@ -2206,10 +2206,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B141" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C141">
         <v>2022</v>
@@ -2217,10 +2217,10 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B142" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C142">
         <v>2022</v>
@@ -2228,70 +2228,150 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B143" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C143">
         <v>2022</v>
-      </c>
-      <c r="D143">
-        <v>2023</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B144" t="s">
+        <v>18</v>
+      </c>
+      <c r="C144">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>55</v>
+      </c>
+      <c r="B145" t="s">
+        <v>19</v>
+      </c>
+      <c r="C145">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>55</v>
+      </c>
+      <c r="B146" t="s">
+        <v>20</v>
+      </c>
+      <c r="C146">
+        <v>2022</v>
+      </c>
+      <c r="D146">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>55</v>
+      </c>
+      <c r="B147" t="s">
+        <v>21</v>
+      </c>
+      <c r="C147">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>55</v>
+      </c>
+      <c r="B148" t="s">
+        <v>24</v>
+      </c>
+      <c r="C148">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>55</v>
+      </c>
+      <c r="B149" t="s">
+        <v>25</v>
+      </c>
+      <c r="C149">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>55</v>
+      </c>
+      <c r="B150" t="s">
+        <v>26</v>
+      </c>
+      <c r="C150">
+        <v>2022</v>
+      </c>
+      <c r="D150">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>55</v>
+      </c>
+      <c r="B151" t="s">
+        <v>59</v>
+      </c>
+      <c r="C151">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>55</v>
+      </c>
+      <c r="B152" t="s">
         <v>60</v>
       </c>
-      <c r="C144">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
-        <v>56</v>
-      </c>
-      <c r="B145" t="s">
-        <v>61</v>
-      </c>
-      <c r="C145">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>56</v>
-      </c>
-      <c r="B146" t="s">
+      <c r="C152">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>55</v>
+      </c>
+      <c r="B153" t="s">
         <v>27</v>
       </c>
-      <c r="C146">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>56</v>
-      </c>
-      <c r="B147" t="s">
+      <c r="C153">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>55</v>
+      </c>
+      <c r="B154" t="s">
         <v>30</v>
       </c>
-      <c r="C147">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
-        <v>56</v>
-      </c>
-      <c r="B148" t="s">
+      <c r="C154">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>55</v>
+      </c>
+      <c r="B155" t="s">
         <v>31</v>
       </c>
-      <c r="C148">
+      <c r="C155">
         <v>2022</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Evaluate timetable using fitness function & improve excel timetable style
</commit_message>
<xml_diff>
--- a/src/main/resources/file/ProgrammeDetails.xlsx
+++ b/src/main/resources/file/ProgrammeDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BA52C2-2EB9-46F1-9E1B-9188639516CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BADACA9-EDE3-41E7-ADCE-FCCA5F90E730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2388C57-8624-4C34-9FA2-70B15EFCE8BC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A2388C57-8624-4C34-9FA2-70B15EFCE8BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>